<commit_message>
Last commit before going to generator for maps
</commit_message>
<xml_diff>
--- a/docs/existingcomponents.xlsx
+++ b/docs/existingcomponents.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>this is a list of existing widgets, etc, from whatever source, for harvesting</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Graphviz integration</t>
+  </si>
+  <si>
+    <t>file upload</t>
+  </si>
+  <si>
+    <t>http://www.swi-prolog.org/howto/http/FileUpload.html</t>
   </si>
 </sst>
 </file>
@@ -453,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,6 +642,20 @@
       </c>
       <c r="D12" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>